<commit_message>
Fiz uma possivel tabela para o relatorio
</commit_message>
<xml_diff>
--- a/Modelo de tabela.xlsx
+++ b/Modelo de tabela.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabrielmizuno/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabrielmizuno/Desktop/EST_aplicada/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{86A46CF1-3346-8240-947C-F7FC2D905B12}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE7BE1E1-3B8D-5847-A785-3F85D99F37A5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{AD32944C-2423-5346-898C-06BC0DE2978C}"/>
+    <workbookView xWindow="8620" yWindow="460" windowWidth="17680" windowHeight="16020" xr2:uid="{AD32944C-2423-5346-898C-06BC0DE2978C}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -20,20 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="11">
-  <si>
-    <t>Variavel 1</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
   <si>
     <t>Sim</t>
   </si>
@@ -41,12 +33,6 @@
     <t xml:space="preserve">Não </t>
   </si>
   <si>
-    <t>Talvez</t>
-  </si>
-  <si>
-    <t>Variavel 2</t>
-  </si>
-  <si>
     <t>Masculino</t>
   </si>
   <si>
@@ -63,6 +49,78 @@
   </si>
   <si>
     <t>P-Valor</t>
+  </si>
+  <si>
+    <t>Sexo</t>
+  </si>
+  <si>
+    <t>Nome no SERASA</t>
+  </si>
+  <si>
+    <t>37.8</t>
+  </si>
+  <si>
+    <t>60.2</t>
+  </si>
+  <si>
+    <t>39.8</t>
+  </si>
+  <si>
+    <t>48.9</t>
+  </si>
+  <si>
+    <t>35.1</t>
+  </si>
+  <si>
+    <t>64.9</t>
+  </si>
+  <si>
+    <t>Casado</t>
+  </si>
+  <si>
+    <t>Solteiro</t>
+  </si>
+  <si>
+    <t>Viuvo</t>
+  </si>
+  <si>
+    <t>Outros</t>
+  </si>
+  <si>
+    <t>Estado civil</t>
+  </si>
+  <si>
+    <t>40.4</t>
+  </si>
+  <si>
+    <t>59.6</t>
+  </si>
+  <si>
+    <t>52.5</t>
+  </si>
+  <si>
+    <t>47.5</t>
+  </si>
+  <si>
+    <t>31.1</t>
+  </si>
+  <si>
+    <t>60.5</t>
+  </si>
+  <si>
+    <t>39.5</t>
+  </si>
+  <si>
+    <t>36.1</t>
+  </si>
+  <si>
+    <t>63.9</t>
+  </si>
+  <si>
+    <t>18.9</t>
+  </si>
+  <si>
+    <t>51.1</t>
   </si>
 </sst>
 </file>
@@ -92,7 +150,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="42">
     <border>
       <left/>
       <right/>
@@ -153,28 +211,6 @@
       <left style="thick">
         <color auto="1"/>
       </left>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color auto="1"/>
-      </left>
-      <right style="thick">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thick">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right/>
       <top/>
       <bottom style="thick">
@@ -351,12 +387,275 @@
       <diagonal style="dashDot">
         <color auto="1"/>
       </diagonal>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="mediumDashDot">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="mediumDashDot">
+        <color auto="1"/>
+      </top>
+      <bottom style="mediumDashed">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="mediumDashed">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="dashDotDot">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dashDotDot">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dashDotDot">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dashDotDot">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -364,49 +663,49 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
@@ -418,19 +717,87 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -747,15 +1114,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C1D9366-A3F4-DA45-BD71-E711FF125797}">
-  <dimension ref="C3:I16"/>
+  <dimension ref="C3:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="18.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="3" spans="3:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -764,153 +1134,241 @@
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="3:9" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="23"/>
+    <row r="4" spans="3:10" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C4" s="21"/>
       <c r="D4" s="3"/>
       <c r="E4" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>4</v>
+        <v>8</v>
+      </c>
+      <c r="F4" s="41" t="s">
+        <v>8</v>
       </c>
       <c r="G4" s="5"/>
       <c r="H4" s="2"/>
-      <c r="I4" s="6"/>
+      <c r="I4" s="35"/>
+      <c r="J4" s="6"/>
     </row>
-    <row r="5" spans="3:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="24"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="16" t="s">
+    <row r="5" spans="3:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C5" s="22"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="42" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" s="15"/>
+      <c r="H5" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="I5" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="3:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C6" s="23"/>
+      <c r="D6" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="G5" s="17"/>
-      <c r="H5" s="7" t="s">
+      <c r="F6" s="43" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="I6" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="J6" s="8"/>
+    </row>
+    <row r="7" spans="3:10" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="C7" s="16" t="s">
         <v>9</v>
-      </c>
-      <c r="I5" s="8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="3:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C6" s="25"/>
-      <c r="D6" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="F6" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="G6" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="H6" s="7"/>
-      <c r="I6" s="8"/>
-    </row>
-    <row r="7" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C7" s="18" t="s">
-        <v>0</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="9"/>
+      <c r="H7" s="39"/>
+      <c r="I7" s="48"/>
+      <c r="J7" s="40"/>
     </row>
-    <row r="8" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C8" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" s="25">
+        <v>37</v>
+      </c>
+      <c r="E8" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="26">
+        <v>56</v>
+      </c>
+      <c r="G8" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" s="24">
+        <v>93</v>
+      </c>
+      <c r="I8" s="49" t="s">
+        <v>13</v>
+      </c>
+      <c r="J8" s="9"/>
+    </row>
+    <row r="9" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C9" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="9"/>
+      <c r="D9" s="45">
+        <v>63</v>
+      </c>
+      <c r="E9" s="46" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="46" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="H9" s="24">
+        <v>97</v>
+      </c>
+      <c r="I9" s="49" t="s">
+        <v>31</v>
+      </c>
+      <c r="J9" s="9"/>
     </row>
-    <row r="9" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C9" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="9"/>
+    <row r="10" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C10" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="9"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="49"/>
+      <c r="J10" s="9"/>
     </row>
-    <row r="10" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C10" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="9"/>
+    <row r="11" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C11" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="25">
+        <v>34</v>
+      </c>
+      <c r="E11" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" s="26">
+        <v>23</v>
+      </c>
+      <c r="G11" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="H11" s="24">
+        <v>57</v>
+      </c>
+      <c r="I11" s="49">
+        <v>30</v>
+      </c>
+      <c r="J11" s="9"/>
     </row>
-    <row r="11" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C11" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="9"/>
+    <row r="12" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C12" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="32">
+        <v>28</v>
+      </c>
+      <c r="E12" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12" s="33">
+        <v>31</v>
+      </c>
+      <c r="G12" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="H12" s="24">
+        <v>59</v>
+      </c>
+      <c r="I12" s="49" t="s">
+        <v>25</v>
+      </c>
+      <c r="J12" s="9"/>
     </row>
-    <row r="12" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C12" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="9"/>
+    <row r="13" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C13" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="25">
+        <v>15</v>
+      </c>
+      <c r="E13" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="F13" s="26">
+        <v>23</v>
+      </c>
+      <c r="G13" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="H13" s="24">
+        <v>38</v>
+      </c>
+      <c r="I13" s="49">
+        <v>20</v>
+      </c>
+      <c r="J13" s="9"/>
     </row>
-    <row r="13" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C13" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="9"/>
+    <row r="14" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C14" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="32">
+        <v>23</v>
+      </c>
+      <c r="E14" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="F14" s="33">
+        <v>13</v>
+      </c>
+      <c r="G14" s="34" t="s">
+        <v>29</v>
+      </c>
+      <c r="H14" s="24">
+        <v>36</v>
+      </c>
+      <c r="I14" s="49" t="s">
+        <v>30</v>
+      </c>
+      <c r="J14" s="9"/>
     </row>
-    <row r="14" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C14" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="9"/>
+    <row r="15" spans="3:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C15" s="17"/>
+      <c r="D15" s="29"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="31"/>
+      <c r="H15" s="37"/>
+      <c r="I15" s="38"/>
+      <c r="J15" s="12"/>
     </row>
-    <row r="15" spans="3:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C15" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="14"/>
-    </row>
-    <row r="16" spans="3:9" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="3:10" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>

<commit_message>
Fiz mais uma tabela
</commit_message>
<xml_diff>
--- a/Modelo de tabela.xlsx
+++ b/Modelo de tabela.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabrielmizuno/Desktop/EST_aplicada/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE7BE1E1-3B8D-5847-A785-3F85D99F37A5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B766895-0586-F749-955A-3A229EB77718}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8620" yWindow="460" windowWidth="17680" windowHeight="16020" xr2:uid="{AD32944C-2423-5346-898C-06BC0DE2978C}"/>
+    <workbookView xWindow="-200" yWindow="540" windowWidth="17680" windowHeight="16020" xr2:uid="{AD32944C-2423-5346-898C-06BC0DE2978C}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="42">
   <si>
     <t>Sim</t>
   </si>
@@ -51,9 +51,6 @@
     <t>P-Valor</t>
   </si>
   <si>
-    <t>Sexo</t>
-  </si>
-  <si>
     <t>Nome no SERASA</t>
   </si>
   <si>
@@ -121,6 +118,39 @@
   </si>
   <si>
     <t>51.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sexo </t>
+  </si>
+  <si>
+    <t>Não</t>
+  </si>
+  <si>
+    <t>Possui nome no SERASA</t>
+  </si>
+  <si>
+    <t>Satisfeito com limite</t>
+  </si>
+  <si>
+    <t>Banco</t>
+  </si>
+  <si>
+    <t>BB</t>
+  </si>
+  <si>
+    <t>Itau</t>
+  </si>
+  <si>
+    <t>Bradesco</t>
+  </si>
+  <si>
+    <t>Caixa</t>
+  </si>
+  <si>
+    <t>Santander</t>
+  </si>
+  <si>
+    <t>Falou com gerente</t>
   </si>
 </sst>
 </file>
@@ -150,7 +180,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="42">
+  <borders count="48">
     <border>
       <left/>
       <right/>
@@ -259,17 +289,6 @@
       <left style="thick">
         <color auto="1"/>
       </left>
-      <right/>
-      <top style="mediumDashDot">
-        <color auto="1"/>
-      </top>
-      <bottom style="mediumDashed">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right/>
       <top style="mediumDashDot">
         <color auto="1"/>
@@ -569,19 +588,6 @@
         <color indexed="64"/>
       </left>
       <right/>
-      <top style="thick">
-        <color auto="1"/>
-      </top>
-      <bottom style="mediumDashDot">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
       <top style="mediumDashDot">
         <color auto="1"/>
       </top>
@@ -647,6 +653,102 @@
         <color indexed="64"/>
       </top>
       <bottom style="dashDotDot">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="mediumDashDot">
+        <color auto="1"/>
+      </top>
+      <bottom style="mediumDashed">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="dashDot">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dashDot">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dashDot">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dashDot">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -655,7 +757,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -663,6 +765,119 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -672,132 +887,36 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1114,10 +1233,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C1D9366-A3F4-DA45-BD71-E711FF125797}">
-  <dimension ref="C3:J16"/>
+  <dimension ref="C3:J35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1135,241 +1254,447 @@
       <c r="I3" s="1"/>
     </row>
     <row r="4" spans="3:10" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="21"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="4" t="s">
+      <c r="C4" s="15"/>
+      <c r="D4" s="42" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" s="43"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="44"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="29"/>
+      <c r="J4" s="3"/>
+    </row>
+    <row r="5" spans="3:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C5" s="16"/>
+      <c r="D5" s="45" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="46"/>
+      <c r="F5" s="47" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" s="48"/>
+      <c r="H5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I5" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="3:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C6" s="17"/>
+      <c r="D6" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="J6" s="5"/>
+    </row>
+    <row r="7" spans="3:10" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="C7" s="10" t="s">
         <v>8</v>
-      </c>
-      <c r="F4" s="41" t="s">
-        <v>8</v>
-      </c>
-      <c r="G4" s="5"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="35"/>
-      <c r="J4" s="6"/>
-    </row>
-    <row r="5" spans="3:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="22"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="F5" s="42" t="s">
-        <v>3</v>
-      </c>
-      <c r="G5" s="15"/>
-      <c r="H5" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="I5" s="36" t="s">
-        <v>6</v>
-      </c>
-      <c r="J5" s="8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="3:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C6" s="23"/>
-      <c r="D6" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="E6" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="F6" s="43" t="s">
-        <v>4</v>
-      </c>
-      <c r="G6" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="I6" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="J6" s="8"/>
-    </row>
-    <row r="7" spans="3:10" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="C7" s="16" t="s">
-        <v>9</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
-      <c r="H7" s="39"/>
-      <c r="I7" s="48"/>
-      <c r="J7" s="40"/>
+      <c r="H7" s="33"/>
+      <c r="I7" s="40"/>
+      <c r="J7" s="34"/>
     </row>
     <row r="8" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D8" s="25">
+      <c r="D8" s="19">
         <v>37</v>
       </c>
-      <c r="E8" s="26" t="s">
+      <c r="E8" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="20">
+        <v>56</v>
+      </c>
+      <c r="G8" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8" s="18">
+        <v>93</v>
+      </c>
+      <c r="I8" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="26">
-        <v>56</v>
-      </c>
-      <c r="G8" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="H8" s="24">
-        <v>93</v>
-      </c>
-      <c r="I8" s="49" t="s">
+      <c r="J8" s="6"/>
+    </row>
+    <row r="9" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C9" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="37">
+        <v>63</v>
+      </c>
+      <c r="E9" s="38" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="J8" s="9"/>
-    </row>
-    <row r="9" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C9" s="44" t="s">
+      <c r="G9" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="H9" s="60">
+        <v>97</v>
+      </c>
+      <c r="I9" s="60" t="s">
+        <v>30</v>
+      </c>
+      <c r="J9" s="6"/>
+    </row>
+    <row r="10" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C10" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="6"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="54"/>
+      <c r="J10" s="6"/>
+    </row>
+    <row r="11" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C11" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="19">
+        <v>34</v>
+      </c>
+      <c r="E11" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" s="20">
+        <v>23</v>
+      </c>
+      <c r="G11" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="H11" s="18">
+        <v>57</v>
+      </c>
+      <c r="I11" s="41">
+        <v>30</v>
+      </c>
+      <c r="J11" s="6"/>
+    </row>
+    <row r="12" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C12" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="26">
+        <v>28</v>
+      </c>
+      <c r="E12" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12" s="27">
+        <v>31</v>
+      </c>
+      <c r="G12" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="H12" s="18">
+        <v>59</v>
+      </c>
+      <c r="I12" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="J12" s="6"/>
+    </row>
+    <row r="13" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C13" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="19">
+        <v>15</v>
+      </c>
+      <c r="E13" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="F13" s="20">
+        <v>23</v>
+      </c>
+      <c r="G13" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="H13" s="18">
+        <v>38</v>
+      </c>
+      <c r="I13" s="41">
+        <v>20</v>
+      </c>
+      <c r="J13" s="6"/>
+    </row>
+    <row r="14" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C14" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="26">
+        <v>23</v>
+      </c>
+      <c r="E14" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="F14" s="27">
+        <v>13</v>
+      </c>
+      <c r="G14" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="H14" s="18">
+        <v>36</v>
+      </c>
+      <c r="I14" s="41" t="s">
+        <v>29</v>
+      </c>
+      <c r="J14" s="6"/>
+    </row>
+    <row r="15" spans="3:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C15" s="11"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="31"/>
+      <c r="I15" s="32"/>
+      <c r="J15" s="9"/>
+    </row>
+    <row r="16" spans="3:10" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="18" spans="3:10" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="3:10" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C19" s="15"/>
+      <c r="D19" s="42" t="s">
+        <v>33</v>
+      </c>
+      <c r="E19" s="43"/>
+      <c r="F19" s="43"/>
+      <c r="G19" s="44"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="29"/>
+      <c r="J19" s="3"/>
+    </row>
+    <row r="20" spans="3:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C20" s="16"/>
+      <c r="D20" s="45" t="s">
+        <v>0</v>
+      </c>
+      <c r="E20" s="46"/>
+      <c r="F20" s="47" t="s">
+        <v>32</v>
+      </c>
+      <c r="G20" s="48"/>
+      <c r="H20" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I20" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="J20" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="3:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C21" s="17"/>
+      <c r="D21" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="E21" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="F21" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="G21" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="I21" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="J21" s="5"/>
+    </row>
+    <row r="22" spans="3:10" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="C22" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="33"/>
+      <c r="I22" s="40"/>
+      <c r="J22" s="34"/>
+    </row>
+    <row r="23" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C23" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D23" s="19"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="21"/>
+      <c r="H23" s="18"/>
+      <c r="I23" s="41"/>
+      <c r="J23" s="6"/>
+    </row>
+    <row r="24" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C24" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="45">
-        <v>63</v>
-      </c>
-      <c r="E9" s="46" t="s">
-        <v>15</v>
-      </c>
-      <c r="F9" s="46" t="s">
-        <v>14</v>
-      </c>
-      <c r="G9" s="47" t="s">
-        <v>10</v>
-      </c>
-      <c r="H9" s="24">
-        <v>97</v>
-      </c>
-      <c r="I9" s="49" t="s">
-        <v>31</v>
-      </c>
-      <c r="J9" s="9"/>
-    </row>
-    <row r="10" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C10" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="9"/>
-      <c r="E10" s="28"/>
-      <c r="F10" s="28"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="24"/>
-      <c r="I10" s="49"/>
-      <c r="J10" s="9"/>
-    </row>
-    <row r="11" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C11" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" s="25">
-        <v>34</v>
-      </c>
-      <c r="E11" s="26" t="s">
-        <v>21</v>
-      </c>
-      <c r="F11" s="26">
-        <v>23</v>
-      </c>
-      <c r="G11" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="H11" s="24">
-        <v>57</v>
-      </c>
-      <c r="I11" s="49">
-        <v>30</v>
-      </c>
-      <c r="J11" s="9"/>
-    </row>
-    <row r="12" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C12" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" s="32">
-        <v>28</v>
-      </c>
-      <c r="E12" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="F12" s="33">
-        <v>31</v>
-      </c>
-      <c r="G12" s="34" t="s">
-        <v>24</v>
-      </c>
-      <c r="H12" s="24">
-        <v>59</v>
-      </c>
-      <c r="I12" s="49" t="s">
-        <v>25</v>
-      </c>
-      <c r="J12" s="9"/>
-    </row>
-    <row r="13" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C13" s="10" t="s">
+      <c r="D24" s="37"/>
+      <c r="E24" s="38"/>
+      <c r="F24" s="38"/>
+      <c r="G24" s="39"/>
+      <c r="H24" s="60"/>
+      <c r="I24" s="60"/>
+      <c r="J24" s="6"/>
+    </row>
+    <row r="25" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C25" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D25" s="6"/>
+      <c r="E25" s="22"/>
+      <c r="F25" s="22"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="8"/>
+      <c r="I25" s="54"/>
+      <c r="J25" s="6"/>
+    </row>
+    <row r="26" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C26" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D26" s="19"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="21"/>
+      <c r="H26" s="18"/>
+      <c r="I26" s="41"/>
+      <c r="J26" s="6"/>
+    </row>
+    <row r="27" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C27" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D27" s="26"/>
+      <c r="E27" s="27"/>
+      <c r="F27" s="27"/>
+      <c r="G27" s="28"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="41"/>
+      <c r="J27" s="6"/>
+    </row>
+    <row r="28" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C28" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D28" s="19"/>
+      <c r="E28" s="20"/>
+      <c r="F28" s="20"/>
+      <c r="G28" s="21"/>
+      <c r="H28" s="18"/>
+      <c r="I28" s="41"/>
+      <c r="J28" s="6"/>
+    </row>
+    <row r="29" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C29" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D29" s="26"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="28"/>
+      <c r="H29" s="41"/>
+      <c r="I29" s="41"/>
+      <c r="J29" s="6"/>
+    </row>
+    <row r="30" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C30" s="49" t="s">
+        <v>40</v>
+      </c>
+      <c r="H30" s="51"/>
+      <c r="I30" s="53"/>
+    </row>
+    <row r="31" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C31" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="25">
-        <v>15</v>
-      </c>
-      <c r="E13" s="26" t="s">
-        <v>26</v>
-      </c>
-      <c r="F13" s="26">
-        <v>23</v>
-      </c>
-      <c r="G13" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="H13" s="24">
-        <v>38</v>
-      </c>
-      <c r="I13" s="49">
-        <v>20</v>
-      </c>
-      <c r="J13" s="9"/>
-    </row>
-    <row r="14" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C14" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="D14" s="32">
-        <v>23</v>
-      </c>
-      <c r="E14" s="33" t="s">
-        <v>28</v>
-      </c>
-      <c r="F14" s="33">
-        <v>13</v>
-      </c>
-      <c r="G14" s="34" t="s">
-        <v>29</v>
-      </c>
-      <c r="H14" s="24">
-        <v>36</v>
-      </c>
-      <c r="I14" s="49" t="s">
-        <v>30</v>
-      </c>
-      <c r="J14" s="9"/>
-    </row>
-    <row r="15" spans="3:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C15" s="17"/>
-      <c r="D15" s="29"/>
-      <c r="E15" s="30"/>
-      <c r="F15" s="30"/>
-      <c r="G15" s="31"/>
-      <c r="H15" s="37"/>
-      <c r="I15" s="38"/>
-      <c r="J15" s="12"/>
-    </row>
-    <row r="16" spans="3:10" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+      <c r="D31" s="57"/>
+      <c r="E31" s="58"/>
+      <c r="F31" s="58"/>
+      <c r="G31" s="58"/>
+      <c r="H31" s="59"/>
+      <c r="I31" s="59"/>
+    </row>
+    <row r="32" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C32" s="49" t="s">
+        <v>41</v>
+      </c>
+      <c r="D32" s="55"/>
+      <c r="E32" s="50"/>
+      <c r="F32" s="50"/>
+      <c r="G32" s="50"/>
+      <c r="H32" s="52"/>
+      <c r="I32" s="52"/>
+    </row>
+    <row r="33" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C33" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="H33" s="52"/>
+      <c r="I33" s="52"/>
+    </row>
+    <row r="34" spans="3:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C34" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D34" s="23"/>
+      <c r="E34" s="24"/>
+      <c r="F34" s="24"/>
+      <c r="G34" s="25"/>
+      <c r="H34" s="31"/>
+      <c r="I34" s="32"/>
+      <c r="J34" s="9"/>
+    </row>
+    <row r="35" spans="3:10" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="D19:G19"/>
+  </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fiz um grafico e mudei a tabela
</commit_message>
<xml_diff>
--- a/Modelo de tabela.xlsx
+++ b/Modelo de tabela.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabrielmizuno/Desktop/EST_aplicada/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B766895-0586-F749-955A-3A229EB77718}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{352AD750-75EE-E046-9EA8-C11131570370}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-200" yWindow="540" windowWidth="17680" windowHeight="16020" xr2:uid="{AD32944C-2423-5346-898C-06BC0DE2978C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{AD32944C-2423-5346-898C-06BC0DE2978C}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="46">
   <si>
     <t>Sim</t>
   </si>
@@ -151,6 +151,18 @@
   </si>
   <si>
     <t>Falou com gerente</t>
+  </si>
+  <si>
+    <t>Layout</t>
+  </si>
+  <si>
+    <t>Confuso</t>
+  </si>
+  <si>
+    <t>Indiferente</t>
+  </si>
+  <si>
+    <t>Bom</t>
   </si>
 </sst>
 </file>
@@ -180,7 +192,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="48">
+  <borders count="53">
     <border>
       <left/>
       <right/>
@@ -749,6 +761,61 @@
         <color indexed="64"/>
       </top>
       <bottom style="dashDot">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="dashDotDot">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="dashDotDot">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -757,7 +824,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -876,27 +943,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -919,6 +965,47 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1233,10 +1320,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C1D9366-A3F4-DA45-BD71-E711FF125797}">
-  <dimension ref="C3:J35"/>
+  <dimension ref="C3:J39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="Q23" sqref="Q23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1255,26 +1342,26 @@
     </row>
     <row r="4" spans="3:10" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C4" s="15"/>
-      <c r="D4" s="42" t="s">
+      <c r="D4" s="54" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="43"/>
-      <c r="F4" s="43"/>
-      <c r="G4" s="44"/>
+      <c r="E4" s="55"/>
+      <c r="F4" s="55"/>
+      <c r="G4" s="56"/>
       <c r="H4" s="2"/>
       <c r="I4" s="29"/>
       <c r="J4" s="3"/>
     </row>
     <row r="5" spans="3:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C5" s="16"/>
-      <c r="D5" s="45" t="s">
+      <c r="D5" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="46"/>
-      <c r="F5" s="47" t="s">
+      <c r="E5" s="58"/>
+      <c r="F5" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="48"/>
+      <c r="G5" s="60"/>
       <c r="H5" s="4" t="s">
         <v>6</v>
       </c>
@@ -1359,10 +1446,10 @@
       <c r="G9" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="H9" s="60">
+      <c r="H9" s="53">
         <v>97</v>
       </c>
-      <c r="I9" s="60" t="s">
+      <c r="I9" s="53" t="s">
         <v>30</v>
       </c>
       <c r="J9" s="6"/>
@@ -1376,7 +1463,7 @@
       <c r="F10" s="22"/>
       <c r="G10" s="7"/>
       <c r="H10" s="8"/>
-      <c r="I10" s="54"/>
+      <c r="I10" s="47"/>
       <c r="J10" s="6"/>
     </row>
     <row r="11" spans="3:10" x14ac:dyDescent="0.2">
@@ -1489,26 +1576,26 @@
     <row r="18" spans="3:10" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="19" spans="3:10" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C19" s="15"/>
-      <c r="D19" s="42" t="s">
+      <c r="D19" s="54" t="s">
         <v>33</v>
       </c>
-      <c r="E19" s="43"/>
-      <c r="F19" s="43"/>
-      <c r="G19" s="44"/>
+      <c r="E19" s="55"/>
+      <c r="F19" s="55"/>
+      <c r="G19" s="56"/>
       <c r="H19" s="2"/>
       <c r="I19" s="29"/>
       <c r="J19" s="3"/>
     </row>
     <row r="20" spans="3:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C20" s="16"/>
-      <c r="D20" s="45" t="s">
+      <c r="D20" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="E20" s="46"/>
-      <c r="F20" s="47" t="s">
+      <c r="E20" s="58"/>
+      <c r="F20" s="59" t="s">
         <v>32</v>
       </c>
-      <c r="G20" s="48"/>
+      <c r="G20" s="60"/>
       <c r="H20" s="4" t="s">
         <v>6</v>
       </c>
@@ -1573,8 +1660,8 @@
       <c r="E24" s="38"/>
       <c r="F24" s="38"/>
       <c r="G24" s="39"/>
-      <c r="H24" s="60"/>
-      <c r="I24" s="60"/>
+      <c r="H24" s="53"/>
+      <c r="I24" s="53"/>
       <c r="J24" s="6"/>
     </row>
     <row r="25" spans="3:10" x14ac:dyDescent="0.2">
@@ -1586,7 +1673,7 @@
       <c r="F25" s="22"/>
       <c r="G25" s="7"/>
       <c r="H25" s="8"/>
-      <c r="I25" s="54"/>
+      <c r="I25" s="47"/>
       <c r="J25" s="6"/>
     </row>
     <row r="26" spans="3:10" x14ac:dyDescent="0.2">
@@ -1638,54 +1725,100 @@
       <c r="J29" s="6"/>
     </row>
     <row r="30" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C30" s="49" t="s">
+      <c r="C30" s="42" t="s">
         <v>40</v>
       </c>
-      <c r="H30" s="51"/>
-      <c r="I30" s="53"/>
+      <c r="H30" s="44"/>
+      <c r="I30" s="46"/>
     </row>
     <row r="31" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C31" s="56" t="s">
+      <c r="C31" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="D31" s="57"/>
-      <c r="E31" s="58"/>
-      <c r="F31" s="58"/>
-      <c r="G31" s="58"/>
-      <c r="H31" s="59"/>
-      <c r="I31" s="59"/>
+      <c r="D31" s="50"/>
+      <c r="E31" s="51"/>
+      <c r="F31" s="51"/>
+      <c r="G31" s="51"/>
+      <c r="H31" s="52"/>
+      <c r="I31" s="52"/>
     </row>
     <row r="32" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C32" s="49" t="s">
+      <c r="C32" s="42" t="s">
         <v>41</v>
       </c>
-      <c r="D32" s="55"/>
-      <c r="E32" s="50"/>
-      <c r="F32" s="50"/>
-      <c r="G32" s="50"/>
-      <c r="H32" s="52"/>
-      <c r="I32" s="52"/>
+      <c r="D32" s="48"/>
+      <c r="E32" s="43"/>
+      <c r="F32" s="43"/>
+      <c r="G32" s="43"/>
+      <c r="H32" s="45"/>
+      <c r="I32" s="45"/>
     </row>
     <row r="33" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C33" s="49" t="s">
+      <c r="C33" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="H33" s="52"/>
-      <c r="I33" s="52"/>
-    </row>
-    <row r="34" spans="3:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C34" s="11" t="s">
+      <c r="H33" s="45"/>
+      <c r="I33" s="45"/>
+    </row>
+    <row r="34" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C34" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D34" s="23"/>
-      <c r="E34" s="24"/>
-      <c r="F34" s="24"/>
-      <c r="G34" s="25"/>
-      <c r="H34" s="31"/>
-      <c r="I34" s="32"/>
-      <c r="J34" s="9"/>
-    </row>
-    <row r="35" spans="3:10" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+      <c r="D34" s="19"/>
+      <c r="E34" s="20"/>
+      <c r="F34" s="20"/>
+      <c r="G34" s="21"/>
+      <c r="H34" s="18"/>
+      <c r="I34" s="46"/>
+      <c r="J34" s="6"/>
+    </row>
+    <row r="35" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C35" s="71" t="s">
+        <v>42</v>
+      </c>
+      <c r="D35" s="72"/>
+      <c r="E35" s="73"/>
+      <c r="F35" s="73"/>
+      <c r="G35" s="74"/>
+      <c r="H35" s="75"/>
+      <c r="I35" s="76"/>
+      <c r="J35" s="61"/>
+    </row>
+    <row r="36" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C36" s="42" t="s">
+        <v>43</v>
+      </c>
+      <c r="D36" s="48"/>
+      <c r="E36" s="43"/>
+      <c r="F36" s="43"/>
+      <c r="G36" s="70"/>
+      <c r="I36" s="44"/>
+    </row>
+    <row r="37" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C37" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="D37" s="67"/>
+      <c r="E37" s="68"/>
+      <c r="F37" s="68"/>
+      <c r="G37" s="69"/>
+      <c r="H37" s="61"/>
+      <c r="I37" s="44"/>
+      <c r="J37" s="61"/>
+    </row>
+    <row r="38" spans="3:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C38" s="66" t="s">
+        <v>45</v>
+      </c>
+      <c r="D38" s="63"/>
+      <c r="E38" s="62"/>
+      <c r="F38" s="62"/>
+      <c r="G38" s="64"/>
+      <c r="H38" s="62"/>
+      <c r="I38" s="65"/>
+      <c r="J38" s="62"/>
+    </row>
+    <row r="39" spans="3:10" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="D4:G4"/>

</xml_diff>

<commit_message>
Fiz um summary e botei uma tabela no excel
</commit_message>
<xml_diff>
--- a/Modelo de tabela.xlsx
+++ b/Modelo de tabela.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabrielmizuno/Desktop/EST_aplicada/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{195B6EF1-BAAD-344F-9330-3201899D2FDB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44BA2A30-5358-334F-8CE8-0C4CC412DEA3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11120" yWindow="460" windowWidth="17680" windowHeight="16020" xr2:uid="{AD32944C-2423-5346-898C-06BC0DE2978C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{AD32944C-2423-5346-898C-06BC0DE2978C}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="64">
   <si>
     <t>Sim</t>
   </si>
@@ -158,18 +158,6 @@
     <t>Falou com gerente</t>
   </si>
   <si>
-    <t>Layout</t>
-  </si>
-  <si>
-    <t>Confuso</t>
-  </si>
-  <si>
-    <t>Indiferente</t>
-  </si>
-  <si>
-    <t>Bom</t>
-  </si>
-  <si>
     <t>24.7</t>
   </si>
   <si>
@@ -189,6 +177,51 @@
   </si>
   <si>
     <t>Nào</t>
+  </si>
+  <si>
+    <t>0.0005155</t>
+  </si>
+  <si>
+    <t>0.1882</t>
+  </si>
+  <si>
+    <t>0.5203</t>
+  </si>
+  <si>
+    <t>0.1505</t>
+  </si>
+  <si>
+    <t>0.1366</t>
+  </si>
+  <si>
+    <t>Min</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>1 Quatil</t>
+  </si>
+  <si>
+    <t>2 Quatil</t>
+  </si>
+  <si>
+    <t>3 Quatil</t>
+  </si>
+  <si>
+    <t>Media</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Desvio Padrão </t>
+  </si>
+  <si>
+    <t>Idadde</t>
+  </si>
+  <si>
+    <t>Tempo de uso do Bankline antes do curso</t>
+  </si>
+  <si>
+    <t>Tempo de uso do Bankline depois do curso</t>
   </si>
 </sst>
 </file>
@@ -204,7 +237,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -217,8 +250,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="52">
+  <borders count="58">
     <border>
       <left/>
       <right/>
@@ -807,37 +846,111 @@
       <right style="thick">
         <color auto="1"/>
       </right>
-      <top/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="dashDotDot">
         <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thick">
-        <color auto="1"/>
-      </left>
+      <left/>
       <right style="thick">
         <color auto="1"/>
       </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="dashDotDot">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thick">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
       <bottom style="dashDot">
         <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="dashDotDot">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="dashDotDot">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="dashDotDot">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="dashDotDot">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="dashDotDot">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="dashDotDot">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="dashDotDot">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -845,7 +958,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -874,9 +987,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -932,12 +1042,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -953,9 +1057,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -963,7 +1064,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
@@ -974,27 +1074,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -1006,27 +1085,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1039,10 +1112,87 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1359,15 +1509,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C1D9366-A3F4-DA45-BD71-E711FF125797}">
-  <dimension ref="C3:J39"/>
+  <dimension ref="C3:S39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="S28" sqref="S28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="36.5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="3:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -1380,31 +1533,31 @@
       <c r="I3" s="1"/>
     </row>
     <row r="4" spans="3:10" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="15"/>
-      <c r="D4" s="48" t="s">
+      <c r="C4" s="14"/>
+      <c r="D4" s="81" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="49"/>
-      <c r="F4" s="49"/>
-      <c r="G4" s="50"/>
+      <c r="E4" s="82"/>
+      <c r="F4" s="82"/>
+      <c r="G4" s="83"/>
       <c r="H4" s="2"/>
-      <c r="I4" s="27"/>
+      <c r="I4" s="26"/>
       <c r="J4" s="3"/>
     </row>
     <row r="5" spans="3:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="16"/>
-      <c r="D5" s="51" t="s">
+      <c r="C5" s="15"/>
+      <c r="D5" s="84" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="52"/>
-      <c r="F5" s="53" t="s">
+      <c r="E5" s="85"/>
+      <c r="F5" s="86" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="54"/>
+      <c r="G5" s="87"/>
       <c r="H5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I5" s="28" t="s">
+      <c r="I5" s="27" t="s">
         <v>6</v>
       </c>
       <c r="J5" s="5" t="s">
@@ -1412,17 +1565,17 @@
       </c>
     </row>
     <row r="6" spans="3:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C6" s="17"/>
-      <c r="D6" s="12" t="s">
+      <c r="C6" s="16"/>
+      <c r="D6" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="13" t="s">
+      <c r="E6" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="32" t="s">
+      <c r="F6" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="G6" s="14" t="s">
+      <c r="G6" s="13" t="s">
         <v>5</v>
       </c>
       <c r="H6" s="4" t="s">
@@ -1434,61 +1587,63 @@
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="3:10" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="67" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="30"/>
-      <c r="I7" s="37"/>
-      <c r="J7" s="31"/>
+      <c r="D7" s="68"/>
+      <c r="E7" s="68"/>
+      <c r="F7" s="68"/>
+      <c r="G7" s="68"/>
+      <c r="H7" s="69"/>
+      <c r="I7" s="70"/>
+      <c r="J7" s="71" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="8" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C8" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="D8" s="19">
+        <v>48</v>
+      </c>
+      <c r="D8" s="18">
         <v>37</v>
       </c>
-      <c r="E8" s="20" t="s">
+      <c r="E8" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="20">
+      <c r="F8" s="19">
         <v>56</v>
       </c>
-      <c r="G8" s="21" t="s">
+      <c r="G8" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="H8" s="18">
+      <c r="H8" s="17">
         <v>93</v>
       </c>
-      <c r="I8" s="38" t="s">
+      <c r="I8" s="34" t="s">
         <v>12</v>
       </c>
       <c r="J8" s="6"/>
     </row>
     <row r="9" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C9" s="33" t="s">
+      <c r="C9" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="D9" s="34">
+      <c r="D9" s="31">
         <v>63</v>
       </c>
-      <c r="E9" s="35" t="s">
+      <c r="E9" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="F9" s="35" t="s">
+      <c r="F9" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="G9" s="36" t="s">
+      <c r="G9" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="H9" s="47">
+      <c r="H9" s="42">
         <v>97</v>
       </c>
-      <c r="I9" s="47" t="s">
+      <c r="I9" s="42" t="s">
         <v>30</v>
       </c>
       <c r="J9" s="6"/>
@@ -1498,33 +1653,35 @@
         <v>19</v>
       </c>
       <c r="D10" s="6"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="22"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
       <c r="G10" s="7"/>
       <c r="H10" s="8"/>
-      <c r="I10" s="44"/>
-      <c r="J10" s="6"/>
+      <c r="I10" s="39"/>
+      <c r="J10" s="6" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="11" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C11" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="19">
+      <c r="D11" s="18">
         <v>34</v>
       </c>
-      <c r="E11" s="20" t="s">
+      <c r="E11" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="F11" s="20">
+      <c r="F11" s="19">
         <v>23</v>
       </c>
-      <c r="G11" s="21" t="s">
+      <c r="G11" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="H11" s="18">
+      <c r="H11" s="17">
         <v>57</v>
       </c>
-      <c r="I11" s="38">
+      <c r="I11" s="34">
         <v>30</v>
       </c>
       <c r="J11" s="6"/>
@@ -1533,22 +1690,22 @@
       <c r="C12" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="24">
+      <c r="D12" s="23">
         <v>28</v>
       </c>
-      <c r="E12" s="25" t="s">
+      <c r="E12" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="F12" s="25">
+      <c r="F12" s="24">
         <v>31</v>
       </c>
-      <c r="G12" s="26" t="s">
+      <c r="G12" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="H12" s="18">
+      <c r="H12" s="17">
         <v>59</v>
       </c>
-      <c r="I12" s="38" t="s">
+      <c r="I12" s="34" t="s">
         <v>24</v>
       </c>
       <c r="J12" s="6"/>
@@ -1557,106 +1714,128 @@
       <c r="C13" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="19">
+      <c r="D13" s="18">
         <v>15</v>
       </c>
-      <c r="E13" s="20" t="s">
+      <c r="E13" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="F13" s="20">
+      <c r="F13" s="19">
         <v>23</v>
       </c>
-      <c r="G13" s="21" t="s">
+      <c r="G13" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="H13" s="18">
+      <c r="H13" s="17">
         <v>38</v>
       </c>
-      <c r="I13" s="38">
+      <c r="I13" s="34">
         <v>20</v>
       </c>
       <c r="J13" s="6"/>
     </row>
     <row r="14" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C14" s="33" t="s">
+      <c r="C14" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="D14" s="34">
+      <c r="D14" s="31">
         <v>23</v>
       </c>
-      <c r="E14" s="35" t="s">
+      <c r="E14" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="F14" s="35">
+      <c r="F14" s="32">
         <v>13</v>
       </c>
-      <c r="G14" s="36" t="s">
+      <c r="G14" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="H14" s="68">
+      <c r="H14" s="52">
         <v>36</v>
       </c>
-      <c r="I14" s="68" t="s">
+      <c r="I14" s="52" t="s">
         <v>29</v>
       </c>
       <c r="J14" s="6"/>
     </row>
     <row r="15" spans="3:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C15" s="11"/>
+      <c r="C15" s="10"/>
       <c r="D15" s="9"/>
-      <c r="E15" s="66"/>
-      <c r="F15" s="66"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="67"/>
-      <c r="I15" s="58"/>
+      <c r="E15" s="50"/>
+      <c r="F15" s="50"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="51"/>
+      <c r="I15" s="46"/>
       <c r="J15" s="9"/>
     </row>
     <row r="16" spans="3:10" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="18" spans="3:10" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="19" spans="3:10" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C19" s="15"/>
-      <c r="D19" s="48" t="s">
+    <row r="18" spans="3:19" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="3:19" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C19" s="14"/>
+      <c r="D19" s="81" t="s">
         <v>34</v>
       </c>
-      <c r="E19" s="49"/>
-      <c r="F19" s="49"/>
-      <c r="G19" s="50"/>
+      <c r="E19" s="82"/>
+      <c r="F19" s="82"/>
+      <c r="G19" s="83"/>
       <c r="H19" s="2"/>
-      <c r="I19" s="27"/>
+      <c r="I19" s="26"/>
       <c r="J19" s="3"/>
     </row>
-    <row r="20" spans="3:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C20" s="16"/>
-      <c r="D20" s="51" t="s">
+    <row r="20" spans="3:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C20" s="15"/>
+      <c r="D20" s="84" t="s">
         <v>32</v>
       </c>
-      <c r="E20" s="52"/>
-      <c r="F20" s="53" t="s">
+      <c r="E20" s="85"/>
+      <c r="F20" s="86" t="s">
         <v>0</v>
       </c>
-      <c r="G20" s="54"/>
+      <c r="G20" s="87"/>
       <c r="H20" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I20" s="28" t="s">
+      <c r="I20" s="27" t="s">
         <v>6</v>
       </c>
       <c r="J20" s="5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="21" spans="3:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C21" s="17"/>
-      <c r="D21" s="12" t="s">
+      <c r="L20" s="88"/>
+      <c r="M20" s="50" t="s">
+        <v>54</v>
+      </c>
+      <c r="N20" s="50" t="s">
+        <v>55</v>
+      </c>
+      <c r="O20" s="50" t="s">
+        <v>56</v>
+      </c>
+      <c r="P20" s="50" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q20" s="50" t="s">
+        <v>58</v>
+      </c>
+      <c r="R20" s="50" t="s">
+        <v>59</v>
+      </c>
+      <c r="S20" s="50" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="3:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C21" s="16"/>
+      <c r="D21" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E21" s="13" t="s">
+      <c r="E21" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F21" s="32" t="s">
+      <c r="F21" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="G21" s="14" t="s">
+      <c r="G21" s="13" t="s">
         <v>5</v>
       </c>
       <c r="H21" s="4" t="s">
@@ -1666,346 +1845,426 @@
         <v>5</v>
       </c>
       <c r="J21" s="5"/>
-    </row>
-    <row r="22" spans="3:10" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="C22" s="10" t="s">
+      <c r="L21" s="89" t="s">
+        <v>61</v>
+      </c>
+      <c r="M21" s="1">
+        <v>20</v>
+      </c>
+      <c r="N21" s="1">
+        <v>42</v>
+      </c>
+      <c r="O21" s="1">
+        <v>28</v>
+      </c>
+      <c r="P21" s="1">
+        <v>30</v>
+      </c>
+      <c r="Q21" s="1">
+        <v>32.75</v>
+      </c>
+      <c r="R21" s="1">
+        <v>30.37</v>
+      </c>
+      <c r="S21" s="1">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="22" spans="3:19" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="C22" s="67" t="s">
         <v>33</v>
       </c>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="30"/>
-      <c r="I22" s="37"/>
-      <c r="J22" s="31"/>
-    </row>
-    <row r="23" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="D22" s="68"/>
+      <c r="E22" s="68"/>
+      <c r="F22" s="68"/>
+      <c r="G22" s="68"/>
+      <c r="H22" s="69"/>
+      <c r="I22" s="70"/>
+      <c r="J22" s="71" t="s">
+        <v>51</v>
+      </c>
+      <c r="L22" s="89" t="s">
+        <v>62</v>
+      </c>
+      <c r="M22" s="1">
+        <v>21</v>
+      </c>
+      <c r="N22" s="1">
+        <v>43</v>
+      </c>
+      <c r="O22" s="1">
+        <v>27</v>
+      </c>
+      <c r="P22" s="1">
+        <v>30</v>
+      </c>
+      <c r="Q22" s="1">
+        <v>33.75</v>
+      </c>
+      <c r="R22" s="1">
+        <v>30.28</v>
+      </c>
+      <c r="S22" s="1">
+        <v>4.53</v>
+      </c>
+    </row>
+    <row r="23" spans="3:19" x14ac:dyDescent="0.2">
       <c r="C23" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D23" s="19">
+      <c r="D23" s="18">
         <v>23</v>
       </c>
-      <c r="E23" s="20" t="s">
+      <c r="E23" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="F23" s="19">
+        <v>28</v>
+      </c>
+      <c r="G23" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="H23" s="17">
+        <v>51</v>
+      </c>
+      <c r="I23" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="J23" s="6"/>
+      <c r="L23" s="89" t="s">
+        <v>63</v>
+      </c>
+      <c r="M23" s="1">
+        <v>34</v>
+      </c>
+      <c r="N23" s="1">
+        <v>65</v>
+      </c>
+      <c r="O23" s="1">
+        <v>48</v>
+      </c>
+      <c r="P23" s="1">
+        <v>50</v>
+      </c>
+      <c r="Q23" s="1">
+        <v>51</v>
+      </c>
+      <c r="R23" s="1">
+        <v>49.92</v>
+      </c>
+      <c r="S23" s="1">
+        <v>3.87</v>
+      </c>
+    </row>
+    <row r="24" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="C24" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="D24" s="31">
+        <v>70</v>
+      </c>
+      <c r="E24" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="F24" s="32">
+        <v>69</v>
+      </c>
+      <c r="G24" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="F23" s="20">
-        <v>28</v>
-      </c>
-      <c r="G23" s="21" t="s">
+      <c r="H24" s="42">
+        <v>139</v>
+      </c>
+      <c r="I24" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="H23" s="18">
-        <v>51</v>
-      </c>
-      <c r="I23" s="38" t="s">
-        <v>48</v>
-      </c>
-      <c r="J23" s="6"/>
-    </row>
-    <row r="24" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C24" s="33" t="s">
-        <v>1</v>
-      </c>
-      <c r="D24" s="34">
-        <v>70</v>
-      </c>
-      <c r="E24" s="35" t="s">
-        <v>49</v>
-      </c>
-      <c r="F24" s="35">
-        <v>69</v>
-      </c>
-      <c r="G24" s="36" t="s">
-        <v>50</v>
-      </c>
-      <c r="H24" s="47">
-        <v>139</v>
-      </c>
-      <c r="I24" s="47" t="s">
-        <v>51</v>
-      </c>
       <c r="J24" s="6"/>
-    </row>
-    <row r="25" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C25" s="7" t="s">
+      <c r="L24" s="89"/>
+      <c r="M24" s="1"/>
+      <c r="N24" s="1"/>
+      <c r="O24" s="1"/>
+      <c r="P24" s="1"/>
+      <c r="Q24" s="1"/>
+      <c r="R24" s="1"/>
+      <c r="S24" s="1"/>
+    </row>
+    <row r="25" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="C25" s="72" t="s">
         <v>35</v>
       </c>
-      <c r="D25" s="6"/>
-      <c r="E25" s="22"/>
-      <c r="F25" s="22"/>
-      <c r="G25" s="7"/>
-      <c r="H25" s="8"/>
-      <c r="I25" s="44"/>
-      <c r="J25" s="6"/>
-    </row>
-    <row r="26" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="D25" s="73"/>
+      <c r="E25" s="74"/>
+      <c r="F25" s="74"/>
+      <c r="G25" s="72"/>
+      <c r="H25" s="75"/>
+      <c r="I25" s="76"/>
+      <c r="J25" s="80" t="s">
+        <v>53</v>
+      </c>
+      <c r="L25" s="89"/>
+      <c r="M25" s="1"/>
+      <c r="N25" s="1"/>
+      <c r="O25" s="1"/>
+      <c r="P25" s="1"/>
+      <c r="Q25" s="1"/>
+      <c r="R25" s="1"/>
+      <c r="S25" s="1"/>
+    </row>
+    <row r="26" spans="3:19" x14ac:dyDescent="0.2">
       <c r="C26" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D26" s="19">
+      <c r="D26" s="18">
         <v>17</v>
       </c>
-      <c r="E26" s="20">
+      <c r="E26" s="19">
         <v>33.299999999999997</v>
       </c>
-      <c r="F26" s="20">
+      <c r="F26" s="19">
         <v>36</v>
       </c>
-      <c r="G26" s="26">
+      <c r="G26" s="25">
         <f>100-E26</f>
         <v>66.7</v>
       </c>
-      <c r="H26" s="18">
+      <c r="H26" s="17">
         <f>D26+F26</f>
         <v>53</v>
       </c>
-      <c r="I26" s="38">
+      <c r="I26" s="34">
         <v>27.9</v>
       </c>
       <c r="J26" s="6"/>
     </row>
-    <row r="27" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="3:19" x14ac:dyDescent="0.2">
       <c r="C27" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D27" s="24">
+      <c r="D27" s="23">
         <v>16</v>
       </c>
-      <c r="E27" s="25">
+      <c r="E27" s="24">
         <v>31.4</v>
       </c>
-      <c r="F27" s="25">
+      <c r="F27" s="24">
         <v>43</v>
       </c>
-      <c r="G27" s="26">
-        <f t="shared" ref="G27:G38" si="0">100-E27</f>
+      <c r="G27" s="25">
+        <f t="shared" ref="G27:G34" si="0">100-E27</f>
         <v>68.599999999999994</v>
       </c>
-      <c r="H27" s="18">
-        <f t="shared" ref="H27:H38" si="1">D27+F27</f>
+      <c r="H27" s="17">
+        <f t="shared" ref="H27:H34" si="1">D27+F27</f>
         <v>59</v>
       </c>
-      <c r="I27" s="38">
+      <c r="I27" s="34">
         <v>31.1</v>
       </c>
       <c r="J27" s="6"/>
     </row>
-    <row r="28" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="3:19" x14ac:dyDescent="0.2">
       <c r="C28" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="D28" s="19">
+      <c r="D28" s="18">
         <v>2</v>
       </c>
-      <c r="E28" s="20">
+      <c r="E28" s="19">
         <v>3.9</v>
       </c>
-      <c r="F28" s="20">
+      <c r="F28" s="19">
         <v>8</v>
       </c>
-      <c r="G28" s="26">
+      <c r="G28" s="25">
         <f t="shared" si="0"/>
         <v>96.1</v>
       </c>
-      <c r="H28" s="18">
+      <c r="H28" s="17">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="I28" s="38">
+      <c r="I28" s="34">
         <v>5.3</v>
       </c>
       <c r="J28" s="6"/>
     </row>
-    <row r="29" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="3:19" x14ac:dyDescent="0.2">
       <c r="C29" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="D29" s="24">
+      <c r="D29" s="23">
         <v>8</v>
       </c>
-      <c r="E29" s="25">
+      <c r="E29" s="24">
         <v>15.7</v>
       </c>
-      <c r="F29" s="25">
+      <c r="F29" s="24">
         <v>10</v>
       </c>
-      <c r="G29" s="26">
+      <c r="G29" s="25">
         <f t="shared" si="0"/>
         <v>84.3</v>
       </c>
-      <c r="H29" s="18">
+      <c r="H29" s="17">
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="I29" s="38">
+      <c r="I29" s="34">
         <v>9.5</v>
       </c>
       <c r="J29" s="6"/>
     </row>
-    <row r="30" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C30" s="39" t="s">
+    <row r="30" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="C30" s="35" t="s">
         <v>40</v>
       </c>
-      <c r="D30" s="71">
+      <c r="D30" s="55">
         <v>4</v>
       </c>
-      <c r="E30" s="72">
+      <c r="E30" s="56">
         <v>7.8</v>
       </c>
-      <c r="F30" s="72">
+      <c r="F30" s="56">
         <v>10</v>
       </c>
-      <c r="G30" s="26">
+      <c r="G30" s="25">
         <f t="shared" si="0"/>
         <v>92.2</v>
       </c>
-      <c r="H30" s="18">
+      <c r="H30" s="17">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="I30" s="18">
+      <c r="I30" s="17">
         <v>7.4</v>
       </c>
-    </row>
-    <row r="31" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C31" s="46" t="s">
+      <c r="J30" s="1"/>
+    </row>
+    <row r="31" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="C31" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="D31" s="73">
+      <c r="D31" s="57">
         <v>4</v>
       </c>
-      <c r="E31" s="74">
+      <c r="E31" s="58">
         <v>7.8</v>
       </c>
-      <c r="F31" s="74">
+      <c r="F31" s="58">
         <v>32</v>
       </c>
-      <c r="G31" s="70">
+      <c r="G31" s="54">
         <f t="shared" si="0"/>
         <v>92.2</v>
       </c>
-      <c r="H31" s="47">
+      <c r="H31" s="42">
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-      <c r="I31" s="47">
+      <c r="I31" s="42">
         <v>18.899999999999999</v>
       </c>
-    </row>
-    <row r="32" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C32" s="39" t="s">
+      <c r="J31" s="1"/>
+    </row>
+    <row r="32" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="C32" s="72" t="s">
         <v>41</v>
       </c>
-      <c r="D32" s="75"/>
-      <c r="E32" s="76"/>
-      <c r="F32" s="76"/>
-      <c r="G32" s="69">
+      <c r="D32" s="77"/>
+      <c r="E32" s="78"/>
+      <c r="F32" s="78"/>
+      <c r="G32" s="79"/>
+      <c r="H32" s="75"/>
+      <c r="I32" s="76"/>
+      <c r="J32" s="80" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="33" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C33" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="D33" s="55">
+        <v>28</v>
+      </c>
+      <c r="E33" s="1">
+        <v>31.8</v>
+      </c>
+      <c r="F33" s="56">
+        <v>60</v>
+      </c>
+      <c r="G33" s="25">
         <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-      <c r="H32" s="8"/>
-      <c r="I32" s="44"/>
-    </row>
-    <row r="33" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C33" s="39" t="s">
-        <v>0</v>
-      </c>
-      <c r="G33" s="26">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-      <c r="H33" s="18">
+        <v>68.2</v>
+      </c>
+      <c r="H33" s="17">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I33" s="42"/>
+        <v>88</v>
+      </c>
+      <c r="I33" s="37"/>
     </row>
     <row r="34" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C34" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="D34" s="19"/>
-      <c r="E34" s="20"/>
-      <c r="F34" s="20"/>
-      <c r="G34" s="26">
+        <v>0</v>
+      </c>
+      <c r="D34" s="18">
+        <v>23</v>
+      </c>
+      <c r="E34" s="19">
+        <v>22.5</v>
+      </c>
+      <c r="F34" s="19">
+        <v>79</v>
+      </c>
+      <c r="G34" s="20">
         <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-      <c r="H34" s="18">
+        <v>77.5</v>
+      </c>
+      <c r="H34" s="17">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I34" s="43"/>
+        <v>102</v>
+      </c>
+      <c r="I34" s="38"/>
       <c r="J34" s="6"/>
     </row>
     <row r="35" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C35" s="62" t="s">
-        <v>42</v>
-      </c>
-      <c r="D35" s="63"/>
-      <c r="E35" s="64"/>
-      <c r="F35" s="64"/>
-      <c r="G35" s="36">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-      <c r="H35" s="68">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I35" s="65"/>
-      <c r="J35" s="55"/>
+      <c r="C35" s="59"/>
+      <c r="D35" s="62"/>
+      <c r="E35" s="63"/>
+      <c r="F35" s="63"/>
+      <c r="G35" s="64"/>
+      <c r="H35" s="65"/>
+      <c r="I35" s="61"/>
+      <c r="J35" s="60"/>
     </row>
     <row r="36" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C36" s="39" t="s">
-        <v>43</v>
-      </c>
-      <c r="D36" s="45"/>
-      <c r="E36" s="40"/>
-      <c r="F36" s="40"/>
-      <c r="G36" s="69">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
+      <c r="C36" s="35"/>
+      <c r="D36" s="40"/>
+      <c r="E36" s="36"/>
+      <c r="F36" s="36"/>
+      <c r="G36" s="53"/>
       <c r="H36" s="8"/>
-      <c r="I36" s="41"/>
+      <c r="I36" s="66"/>
     </row>
     <row r="37" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C37" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="D37" s="60"/>
-      <c r="E37" s="61"/>
-      <c r="F37" s="61"/>
-      <c r="G37" s="26">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-      <c r="H37" s="18">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I37" s="41"/>
-      <c r="J37" s="55"/>
+      <c r="C37" s="21"/>
+      <c r="D37" s="48"/>
+      <c r="E37" s="49"/>
+      <c r="F37" s="49"/>
+      <c r="G37" s="25"/>
+      <c r="H37" s="17"/>
+      <c r="I37" s="37"/>
+      <c r="J37" s="43"/>
     </row>
     <row r="38" spans="3:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C38" s="59" t="s">
-        <v>45</v>
-      </c>
-      <c r="D38" s="57"/>
-      <c r="E38" s="56"/>
-      <c r="F38" s="56"/>
-      <c r="G38" s="23">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-      <c r="H38" s="29">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I38" s="58"/>
-      <c r="J38" s="56"/>
+      <c r="C38" s="47"/>
+      <c r="D38" s="45"/>
+      <c r="E38" s="44"/>
+      <c r="F38" s="44"/>
+      <c r="G38" s="22"/>
+      <c r="H38" s="28"/>
+      <c r="I38" s="46"/>
+      <c r="J38" s="44"/>
     </row>
     <row r="39" spans="3:10" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>

</xml_diff>

<commit_message>
Mexi no arquivo doc
</commit_message>
<xml_diff>
--- a/Modelo de tabela.xlsx
+++ b/Modelo de tabela.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabrielmizuno/Desktop/EST_aplicada/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44BA2A30-5358-334F-8CE8-0C4CC412DEA3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74CD8BBE-5C81-0D4D-B969-2421960CFAA2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{AD32944C-2423-5346-898C-06BC0DE2978C}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16020" xr2:uid="{AD32944C-2423-5346-898C-06BC0DE2978C}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="65">
   <si>
     <t>Sim</t>
   </si>
@@ -222,14 +222,25 @@
   </si>
   <si>
     <t>Tempo de uso do Bankline depois do curso</t>
+  </si>
+  <si>
+    <t>`</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -958,7 +969,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1036,9 +1047,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1066,9 +1074,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1168,6 +1173,12 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1189,10 +1200,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1512,7 +1529,7 @@
   <dimension ref="C3:S39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S28" sqref="S28"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1523,7 +1540,7 @@
     <col min="19" max="19" width="13.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -1532,7 +1549,7 @@
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="3:10" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:11" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C4" s="14"/>
       <c r="D4" s="81" t="s">
         <v>31</v>
@@ -1544,7 +1561,7 @@
       <c r="I4" s="26"/>
       <c r="J4" s="3"/>
     </row>
-    <row r="5" spans="3:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C5" s="15"/>
       <c r="D5" s="84" t="s">
         <v>2</v>
@@ -1554,17 +1571,17 @@
         <v>3</v>
       </c>
       <c r="G5" s="87"/>
-      <c r="H5" s="4" t="s">
+      <c r="H5" s="89" t="s">
         <v>6</v>
       </c>
-      <c r="I5" s="27" t="s">
+      <c r="I5" s="90" t="s">
         <v>6</v>
       </c>
-      <c r="J5" s="5" t="s">
+      <c r="J5" s="91" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="3:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C6" s="16"/>
       <c r="D6" s="11" t="s">
         <v>4</v>
@@ -1572,7 +1589,7 @@
       <c r="E6" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="29" t="s">
+      <c r="F6" s="28" t="s">
         <v>4</v>
       </c>
       <c r="G6" s="13" t="s">
@@ -1586,21 +1603,21 @@
       </c>
       <c r="J6" s="5"/>
     </row>
-    <row r="7" spans="3:10" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="C7" s="67" t="s">
+    <row r="7" spans="3:11" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="C7" s="65" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="68"/>
-      <c r="E7" s="68"/>
-      <c r="F7" s="68"/>
-      <c r="G7" s="68"/>
-      <c r="H7" s="69"/>
-      <c r="I7" s="70"/>
-      <c r="J7" s="71" t="s">
+      <c r="D7" s="66"/>
+      <c r="E7" s="66"/>
+      <c r="F7" s="66"/>
+      <c r="G7" s="66"/>
+      <c r="H7" s="67"/>
+      <c r="I7" s="68"/>
+      <c r="J7" s="69" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C8" s="7" t="s">
         <v>48</v>
       </c>
@@ -1619,50 +1636,50 @@
       <c r="H8" s="17">
         <v>93</v>
       </c>
-      <c r="I8" s="34" t="s">
+      <c r="I8" s="33" t="s">
         <v>12</v>
       </c>
       <c r="J8" s="6"/>
     </row>
-    <row r="9" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C9" s="30" t="s">
+    <row r="9" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C9" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="D9" s="31">
+      <c r="D9" s="30">
         <v>63</v>
       </c>
-      <c r="E9" s="32" t="s">
+      <c r="E9" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="F9" s="32" t="s">
+      <c r="F9" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="G9" s="33" t="s">
+      <c r="G9" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="H9" s="42">
+      <c r="H9" s="40">
         <v>97</v>
       </c>
-      <c r="I9" s="42" t="s">
+      <c r="I9" s="40" t="s">
         <v>30</v>
       </c>
       <c r="J9" s="6"/>
     </row>
-    <row r="10" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C10" s="7" t="s">
+    <row r="10" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C10" s="70" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="6"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="39"/>
-      <c r="J10" s="6" t="s">
+      <c r="D10" s="71"/>
+      <c r="E10" s="72"/>
+      <c r="F10" s="72"/>
+      <c r="G10" s="70"/>
+      <c r="H10" s="73"/>
+      <c r="I10" s="74"/>
+      <c r="J10" s="78" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C11" s="7" t="s">
         <v>15</v>
       </c>
@@ -1681,12 +1698,13 @@
       <c r="H11" s="17">
         <v>57</v>
       </c>
-      <c r="I11" s="34">
+      <c r="I11" s="33">
         <v>30</v>
       </c>
       <c r="J11" s="6"/>
-    </row>
-    <row r="12" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="K11" s="41"/>
+    </row>
+    <row r="12" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C12" s="7" t="s">
         <v>16</v>
       </c>
@@ -1705,12 +1723,12 @@
       <c r="H12" s="17">
         <v>59</v>
       </c>
-      <c r="I12" s="34" t="s">
+      <c r="I12" s="33" t="s">
         <v>24</v>
       </c>
       <c r="J12" s="6"/>
     </row>
-    <row r="13" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C13" s="7" t="s">
         <v>17</v>
       </c>
@@ -1729,46 +1747,46 @@
       <c r="H13" s="17">
         <v>38</v>
       </c>
-      <c r="I13" s="34">
+      <c r="I13" s="33">
         <v>20</v>
       </c>
       <c r="J13" s="6"/>
     </row>
-    <row r="14" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C14" s="30" t="s">
+    <row r="14" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C14" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="D14" s="31">
+      <c r="D14" s="30">
         <v>23</v>
       </c>
-      <c r="E14" s="32" t="s">
+      <c r="E14" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="F14" s="32">
+      <c r="F14" s="31">
         <v>13</v>
       </c>
-      <c r="G14" s="33" t="s">
+      <c r="G14" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="H14" s="52">
+      <c r="H14" s="50">
         <v>36</v>
       </c>
-      <c r="I14" s="52" t="s">
+      <c r="I14" s="50" t="s">
         <v>29</v>
       </c>
       <c r="J14" s="6"/>
     </row>
-    <row r="15" spans="3:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C15" s="10"/>
       <c r="D15" s="9"/>
-      <c r="E15" s="50"/>
-      <c r="F15" s="50"/>
+      <c r="E15" s="48"/>
+      <c r="F15" s="48"/>
       <c r="G15" s="10"/>
-      <c r="H15" s="51"/>
-      <c r="I15" s="46"/>
+      <c r="H15" s="49"/>
+      <c r="I15" s="44"/>
       <c r="J15" s="9"/>
     </row>
-    <row r="16" spans="3:10" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="3:11" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="18" spans="3:19" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="19" spans="3:19" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C19" s="14"/>
@@ -1792,35 +1810,37 @@
         <v>0</v>
       </c>
       <c r="G20" s="87"/>
-      <c r="H20" s="4" t="s">
+      <c r="H20" s="89" t="s">
         <v>6</v>
       </c>
-      <c r="I20" s="27" t="s">
+      <c r="I20" s="90" t="s">
         <v>6</v>
       </c>
-      <c r="J20" s="5" t="s">
+      <c r="J20" s="91" t="s">
         <v>7</v>
       </c>
-      <c r="L20" s="88"/>
-      <c r="M20" s="50" t="s">
+      <c r="L20" s="79" t="s">
+        <v>64</v>
+      </c>
+      <c r="M20" s="48" t="s">
         <v>54</v>
       </c>
-      <c r="N20" s="50" t="s">
+      <c r="N20" s="48" t="s">
         <v>55</v>
       </c>
-      <c r="O20" s="50" t="s">
+      <c r="O20" s="48" t="s">
         <v>56</v>
       </c>
-      <c r="P20" s="50" t="s">
+      <c r="P20" s="48" t="s">
         <v>57</v>
       </c>
-      <c r="Q20" s="50" t="s">
+      <c r="Q20" s="48" t="s">
         <v>58</v>
       </c>
-      <c r="R20" s="50" t="s">
+      <c r="R20" s="48" t="s">
         <v>59</v>
       </c>
-      <c r="S20" s="50" t="s">
+      <c r="S20" s="48" t="s">
         <v>60</v>
       </c>
     </row>
@@ -1832,7 +1852,7 @@
       <c r="E21" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F21" s="29" t="s">
+      <c r="F21" s="28" t="s">
         <v>4</v>
       </c>
       <c r="G21" s="13" t="s">
@@ -1845,7 +1865,7 @@
         <v>5</v>
       </c>
       <c r="J21" s="5"/>
-      <c r="L21" s="89" t="s">
+      <c r="L21" s="80" t="s">
         <v>61</v>
       </c>
       <c r="M21" s="1">
@@ -1871,19 +1891,19 @@
       </c>
     </row>
     <row r="22" spans="3:19" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="C22" s="67" t="s">
+      <c r="C22" s="65" t="s">
         <v>33</v>
       </c>
-      <c r="D22" s="68"/>
-      <c r="E22" s="68"/>
-      <c r="F22" s="68"/>
-      <c r="G22" s="68"/>
-      <c r="H22" s="69"/>
-      <c r="I22" s="70"/>
-      <c r="J22" s="71" t="s">
+      <c r="D22" s="66"/>
+      <c r="E22" s="66"/>
+      <c r="F22" s="66"/>
+      <c r="G22" s="66"/>
+      <c r="H22" s="67"/>
+      <c r="I22" s="68"/>
+      <c r="J22" s="69" t="s">
         <v>51</v>
       </c>
-      <c r="L22" s="89" t="s">
+      <c r="L22" s="80" t="s">
         <v>62</v>
       </c>
       <c r="M22" s="1">
@@ -1927,11 +1947,11 @@
       <c r="H23" s="17">
         <v>51</v>
       </c>
-      <c r="I23" s="34" t="s">
+      <c r="I23" s="33" t="s">
         <v>44</v>
       </c>
       <c r="J23" s="6"/>
-      <c r="L23" s="89" t="s">
+      <c r="L23" s="80" t="s">
         <v>63</v>
       </c>
       <c r="M23" s="1">
@@ -1957,29 +1977,29 @@
       </c>
     </row>
     <row r="24" spans="3:19" x14ac:dyDescent="0.2">
-      <c r="C24" s="30" t="s">
+      <c r="C24" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="D24" s="31">
+      <c r="D24" s="30">
         <v>70</v>
       </c>
-      <c r="E24" s="32" t="s">
+      <c r="E24" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="F24" s="32">
+      <c r="F24" s="31">
         <v>69</v>
       </c>
-      <c r="G24" s="33" t="s">
+      <c r="G24" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="H24" s="42">
+      <c r="H24" s="40">
         <v>139</v>
       </c>
-      <c r="I24" s="42" t="s">
+      <c r="I24" s="40" t="s">
         <v>47</v>
       </c>
       <c r="J24" s="6"/>
-      <c r="L24" s="89"/>
+      <c r="L24" s="88"/>
       <c r="M24" s="1"/>
       <c r="N24" s="1"/>
       <c r="O24" s="1"/>
@@ -1989,19 +2009,19 @@
       <c r="S24" s="1"/>
     </row>
     <row r="25" spans="3:19" x14ac:dyDescent="0.2">
-      <c r="C25" s="72" t="s">
+      <c r="C25" s="70" t="s">
         <v>35</v>
       </c>
-      <c r="D25" s="73"/>
-      <c r="E25" s="74"/>
-      <c r="F25" s="74"/>
-      <c r="G25" s="72"/>
-      <c r="H25" s="75"/>
-      <c r="I25" s="76"/>
-      <c r="J25" s="80" t="s">
+      <c r="D25" s="71"/>
+      <c r="E25" s="72"/>
+      <c r="F25" s="72"/>
+      <c r="G25" s="70"/>
+      <c r="H25" s="73"/>
+      <c r="I25" s="74"/>
+      <c r="J25" s="78" t="s">
         <v>53</v>
       </c>
-      <c r="L25" s="89"/>
+      <c r="L25" s="88"/>
       <c r="M25" s="1"/>
       <c r="N25" s="1"/>
       <c r="O25" s="1"/>
@@ -2031,7 +2051,7 @@
         <f>D26+F26</f>
         <v>53</v>
       </c>
-      <c r="I26" s="34">
+      <c r="I26" s="33">
         <v>27.9</v>
       </c>
       <c r="J26" s="6"/>
@@ -2057,7 +2077,7 @@
         <f t="shared" ref="H27:H34" si="1">D27+F27</f>
         <v>59</v>
       </c>
-      <c r="I27" s="34">
+      <c r="I27" s="33">
         <v>31.1</v>
       </c>
       <c r="J27" s="6"/>
@@ -2083,7 +2103,7 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="I28" s="34">
+      <c r="I28" s="33">
         <v>5.3</v>
       </c>
       <c r="J28" s="6"/>
@@ -2109,22 +2129,22 @@
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="I29" s="34">
+      <c r="I29" s="33">
         <v>9.5</v>
       </c>
       <c r="J29" s="6"/>
     </row>
     <row r="30" spans="3:19" x14ac:dyDescent="0.2">
-      <c r="C30" s="35" t="s">
+      <c r="C30" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="D30" s="55">
+      <c r="D30" s="53">
         <v>4</v>
       </c>
-      <c r="E30" s="56">
+      <c r="E30" s="54">
         <v>7.8</v>
       </c>
-      <c r="F30" s="56">
+      <c r="F30" s="54">
         <v>10</v>
       </c>
       <c r="G30" s="25">
@@ -2141,56 +2161,56 @@
       <c r="J30" s="1"/>
     </row>
     <row r="31" spans="3:19" x14ac:dyDescent="0.2">
-      <c r="C31" s="41" t="s">
+      <c r="C31" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="D31" s="57">
+      <c r="D31" s="55">
         <v>4</v>
       </c>
-      <c r="E31" s="58">
+      <c r="E31" s="56">
         <v>7.8</v>
       </c>
-      <c r="F31" s="58">
+      <c r="F31" s="56">
         <v>32</v>
       </c>
-      <c r="G31" s="54">
+      <c r="G31" s="52">
         <f t="shared" si="0"/>
         <v>92.2</v>
       </c>
-      <c r="H31" s="42">
+      <c r="H31" s="40">
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-      <c r="I31" s="42">
+      <c r="I31" s="40">
         <v>18.899999999999999</v>
       </c>
       <c r="J31" s="1"/>
     </row>
     <row r="32" spans="3:19" x14ac:dyDescent="0.2">
-      <c r="C32" s="72" t="s">
+      <c r="C32" s="70" t="s">
         <v>41</v>
       </c>
-      <c r="D32" s="77"/>
-      <c r="E32" s="78"/>
-      <c r="F32" s="78"/>
-      <c r="G32" s="79"/>
-      <c r="H32" s="75"/>
-      <c r="I32" s="76"/>
-      <c r="J32" s="80" t="s">
+      <c r="D32" s="75"/>
+      <c r="E32" s="76"/>
+      <c r="F32" s="76"/>
+      <c r="G32" s="77"/>
+      <c r="H32" s="73"/>
+      <c r="I32" s="74"/>
+      <c r="J32" s="78" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="33" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C33" s="35" t="s">
+      <c r="C33" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="D33" s="55">
+      <c r="D33" s="53">
         <v>28</v>
       </c>
       <c r="E33" s="1">
         <v>31.8</v>
       </c>
-      <c r="F33" s="56">
+      <c r="F33" s="54">
         <v>60</v>
       </c>
       <c r="G33" s="25">
@@ -2201,7 +2221,7 @@
         <f t="shared" si="1"/>
         <v>88</v>
       </c>
-      <c r="I33" s="37"/>
+      <c r="I33" s="36"/>
     </row>
     <row r="34" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C34" s="7" t="s">
@@ -2224,47 +2244,47 @@
         <f t="shared" si="1"/>
         <v>102</v>
       </c>
-      <c r="I34" s="38"/>
+      <c r="I34" s="37"/>
       <c r="J34" s="6"/>
     </row>
     <row r="35" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C35" s="59"/>
-      <c r="D35" s="62"/>
-      <c r="E35" s="63"/>
-      <c r="F35" s="63"/>
-      <c r="G35" s="64"/>
-      <c r="H35" s="65"/>
-      <c r="I35" s="61"/>
-      <c r="J35" s="60"/>
+      <c r="C35" s="57"/>
+      <c r="D35" s="60"/>
+      <c r="E35" s="61"/>
+      <c r="F35" s="61"/>
+      <c r="G35" s="62"/>
+      <c r="H35" s="63"/>
+      <c r="I35" s="59"/>
+      <c r="J35" s="58"/>
     </row>
     <row r="36" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C36" s="35"/>
-      <c r="D36" s="40"/>
-      <c r="E36" s="36"/>
-      <c r="F36" s="36"/>
-      <c r="G36" s="53"/>
+      <c r="C36" s="34"/>
+      <c r="D36" s="38"/>
+      <c r="E36" s="35"/>
+      <c r="F36" s="35"/>
+      <c r="G36" s="51"/>
       <c r="H36" s="8"/>
-      <c r="I36" s="66"/>
+      <c r="I36" s="64"/>
     </row>
     <row r="37" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C37" s="21"/>
-      <c r="D37" s="48"/>
-      <c r="E37" s="49"/>
-      <c r="F37" s="49"/>
+      <c r="D37" s="46"/>
+      <c r="E37" s="47"/>
+      <c r="F37" s="47"/>
       <c r="G37" s="25"/>
       <c r="H37" s="17"/>
-      <c r="I37" s="37"/>
-      <c r="J37" s="43"/>
+      <c r="I37" s="36"/>
+      <c r="J37" s="41"/>
     </row>
     <row r="38" spans="3:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C38" s="47"/>
-      <c r="D38" s="45"/>
-      <c r="E38" s="44"/>
-      <c r="F38" s="44"/>
+      <c r="C38" s="45"/>
+      <c r="D38" s="43"/>
+      <c r="E38" s="42"/>
+      <c r="F38" s="42"/>
       <c r="G38" s="22"/>
-      <c r="H38" s="28"/>
-      <c r="I38" s="46"/>
-      <c r="J38" s="44"/>
+      <c r="H38" s="27"/>
+      <c r="I38" s="44"/>
+      <c r="J38" s="42"/>
     </row>
     <row r="39" spans="3:10" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>

</xml_diff>